<commit_message>
date range for download report
</commit_message>
<xml_diff>
--- a/code list.xlsx
+++ b/code list.xlsx
@@ -411,7 +411,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -426,7 +426,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -436,7 +436,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A.P.10</t>
+          <t>ACS10</t>
         </is>
       </c>
     </row>
@@ -448,7 +448,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -463,7 +463,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>A.P.20</t>
+          <t>ACS20</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>A.P.3</t>
+          <t>ACS3</t>
         </is>
       </c>
     </row>
@@ -522,7 +522,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>A.P.4</t>
+          <t>ACS4</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -584,7 +584,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A.P.5</t>
+          <t>ACS5</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>A.P.6</t>
+          <t>ACS6</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -658,7 +658,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>A.P.7</t>
+          <t>ACS7</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>konsumen</t>
+          <t>customer</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A.P.8</t>
+          <t>ACS8</t>
         </is>
       </c>
     </row>
@@ -732,7 +732,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>A.PO.2</t>
+          <t>APO2</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>A.PO.3</t>
+          <t>APO3</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>layanan</t>
+          <t>service</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>A.S.1</t>
+          <t>AS1</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>layanan</t>
+          <t>service</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -843,7 +843,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>A.S.2</t>
+          <t>AS2</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>layanan</t>
+          <t>service</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>A.S.3</t>
+          <t>AS3</t>
         </is>
       </c>
     </row>
@@ -917,7 +917,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>B.NF.1</t>
+          <t>BNF1</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>B.NF.2</t>
+          <t>BNF2</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>B.NF.3</t>
+          <t>BNF3</t>
         </is>
       </c>
     </row>

</xml_diff>